<commit_message>
deng pai deng ma
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="81">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -252,6 +252,12 @@
   </si>
   <si>
     <t xml:space="preserve">&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId26</t>
   </si>
 </sst>
 </file>
@@ -1833,7 +1839,7 @@
     </row>
     <row r="11">
       <c r="B11" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -1845,12 +1851,12 @@
         <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -1862,15 +1868,15 @@
         <v>44</v>
       </c>
       <c r="F12" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>57</v>
@@ -1879,12 +1885,12 @@
         <v>44</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
@@ -1896,15 +1902,15 @@
         <v>44</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
         <v>57</v>
@@ -1918,7 +1924,7 @@
     </row>
     <row r="16">
       <c r="B16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1930,12 +1936,12 @@
         <v>44</v>
       </c>
       <c r="F16" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C17" t="s">
         <v>38</v>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
@@ -1964,12 +1970,12 @@
         <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1981,24 +1987,41 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E20" t="s">
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>52</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="B21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add left right wall
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="790" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1406" uniqueCount="87">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -258,6 +258,24 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">score &lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score&lt;value&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Score&lt;10&gt;</t>
   </si>
 </sst>
 </file>
@@ -1958,13 +1976,13 @@
     </row>
     <row r="18">
       <c r="B18" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="C18" t="s">
         <v>38</v>
       </c>
       <c r="D18" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
         <v>44</v>
@@ -1975,7 +1993,7 @@
     </row>
     <row r="19">
       <c r="B19" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
@@ -1987,43 +2005,29 @@
         <v>44</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C20" t="s">
         <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
         <v>44</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="B21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s">
-        <v>38</v>
-      </c>
-      <c r="D21" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F21" t="s">
-        <v>58</v>
-      </c>
-    </row>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
fix first msg from uart
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2631" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2791" uniqueCount="113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -351,6 +351,9 @@
   </si>
   <si>
     <t xml:space="preserve">default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No music</t>
   </si>
 </sst>
 </file>
@@ -2241,7 +2244,7 @@
         <v>44</v>
       </c>
       <c r="F26" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>